<commit_message>
Renamed and moved around some map and graph files. Started on adding a Shiny app which is a line graph of federal voting intentions. Added some public polls to the raw data and updated the main poll dataset.
</commit_message>
<xml_diff>
--- a/Data/Polls/Raw/Federal/raw_0001.xlsx
+++ b/Data/Polls/Raw/Federal/raw_0001.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">pollster</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">Leger</t>
   </si>
   <si>
+    <t xml:space="preserve">https://leger360.com/wp-content/uploads/2021/01/Legers-North-American-Tracker-January-4th-2021-min.pdf?x16723</t>
+  </si>
+  <si>
     <t xml:space="preserve">date</t>
   </si>
   <si>
@@ -49,6 +52,9 @@
     <t xml:space="preserve">BC</t>
   </si>
   <si>
+    <t xml:space="preserve">CAN</t>
+  </si>
+  <si>
     <t xml:space="preserve">LIB</t>
   </si>
   <si>
@@ -71,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">nu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">votesum</t>
   </si>
 </sst>
 </file>
@@ -176,30 +185,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>2</v>
+      <c r="A2" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>44287</v>
@@ -212,27 +223,30 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>48</v>
@@ -252,10 +266,13 @@
       <c r="G4" s="1" t="n">
         <v>35</v>
       </c>
+      <c r="H4" s="1" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>17</v>
@@ -275,10 +292,13 @@
       <c r="G5" s="1" t="n">
         <v>25</v>
       </c>
+      <c r="H5" s="1" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>24</v>
@@ -298,18 +318,24 @@
       <c r="G6" s="1" t="n">
         <v>26</v>
       </c>
+      <c r="H6" s="1" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>30</v>
       </c>
+      <c r="H7" s="1" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>7</v>
@@ -329,10 +355,13 @@
       <c r="G8" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="H8" s="1" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>4</v>
@@ -352,51 +381,93 @@
       <c r="G9" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="H9" s="1" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="0" t="n">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>291</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>471</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>145</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>174</v>
       </c>
+      <c r="H10" s="1" t="n">
+        <v>1506</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="0" t="n">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>325</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="1" t="n">
         <v>109</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <v>127</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>1506</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <f aca="false">SUM(B4:B9)</f>
+        <v>100</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <f aca="false">SUM(C4:C9)</f>
+        <v>100</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <f aca="false">SUM(D4:D9)</f>
+        <v>99</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <f aca="false">SUM(E4:E9)</f>
+        <v>100</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <f aca="false">SUM(F4:F9)</f>
+        <v>100</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <f aca="false">SUM(G4:G9)</f>
+        <v>99</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <f aca="false">SUM(H4:H9)</f>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a poll and amended two old polls
</commit_message>
<xml_diff>
--- a/Data/Polls/Raw/Federal/raw_0001.xlsx
+++ b/Data/Polls/Raw/Federal/raw_0001.xlsx
@@ -188,10 +188,10 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -266,8 +266,8 @@
       <c r="G4" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="H4" s="1" t="n">
-        <v>33</v>
+      <c r="H4" s="0" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -292,8 +292,8 @@
       <c r="G5" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="H5" s="1" t="n">
-        <v>33</v>
+      <c r="H5" s="0" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -318,8 +318,8 @@
       <c r="G6" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="H6" s="1" t="n">
-        <v>18</v>
+      <c r="H6" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -329,8 +329,8 @@
       <c r="C7" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="H7" s="1" t="n">
-        <v>8</v>
+      <c r="H7" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -355,7 +355,7 @@
       <c r="G8" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="H8" s="1" t="n">
+      <c r="H8" s="0" t="n">
         <v>6</v>
       </c>
     </row>
@@ -381,7 +381,7 @@
       <c r="G9" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="H9" s="1" t="n">
+      <c r="H9" s="0" t="n">
         <v>2</v>
       </c>
     </row>
@@ -408,7 +408,7 @@
         <v>174</v>
       </c>
       <c r="H10" s="1" t="n">
-        <v>1506</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -434,7 +434,7 @@
         <v>127</v>
       </c>
       <c r="H11" s="1" t="n">
-        <v>1506</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>